<commit_message>
updates - config, word
updated the config reader to read in more configurable information.
Updated the word doc to add a page at the end of the Pre-Neg that includes any issues and/or errors found in that offer
</commit_message>
<xml_diff>
--- a/FAS PSS New Offer/config.xlsx
+++ b/FAS PSS New Offer/config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -200,6 +200,9 @@
     <t>Shared drive to be used</t>
   </si>
   <si>
+    <t>shareDrive</t>
+  </si>
+  <si>
     <t>certificationError_message</t>
   </si>
   <si>
@@ -224,16 +227,37 @@
     <t>email address to send error email</t>
   </si>
   <si>
+    <t>errorEmailAddress</t>
+  </si>
+  <si>
+    <t>successEmailAddress</t>
+  </si>
+  <si>
     <t>email address to send sucess email</t>
   </si>
   <si>
-    <t>shareDrive_orig</t>
-  </si>
-  <si>
-    <t>errorEmailAddress_orig</t>
-  </si>
-  <si>
-    <t>successEmailAddress_orig</t>
+    <t>MediumTimeSpan</t>
+  </si>
+  <si>
+    <t>2 second time span</t>
+  </si>
+  <si>
+    <t>email address to use in the "from" field</t>
+  </si>
+  <si>
+    <t>fromEmailAddress</t>
+  </si>
+  <si>
+    <t>emailName</t>
+  </si>
+  <si>
+    <t>Truman  GSA</t>
+  </si>
+  <si>
+    <t>"Name" to use for return email</t>
+  </si>
+  <si>
+    <t>00:00:02</t>
   </si>
 </sst>
 </file>
@@ -280,10 +304,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -565,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z990"/>
+  <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -670,40 +695,60 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" t="s">
-        <v>66</v>
-      </c>
-    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1679,11 +1724,9 @@
     <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
-    <hyperlink ref="B12" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1692,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1923,30 +1966,40 @@
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2920,6 +2973,7 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>